<commit_message>
Performed experiments, added image, retrained neural net
</commit_message>
<xml_diff>
--- a/results/comparison.xlsx
+++ b/results/comparison.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephnasante/Desktop/Housing-Price-Prediction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephnasante/Desktop/Housing-Price-Prediction/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Neural Network</t>
   </si>
   <si>
-    <t>Addition of K-Nearest Neighbors</t>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>Combination</t>
   </si>
 </sst>
 </file>
@@ -48,12 +51,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,11 +77,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,29 +192,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$B$1</c:f>
+              <c:f>Sheet1!$A$1:$C$1</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Neural Network</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Addition of K-Nearest Neighbors</c:v>
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Combination</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$B$2</c:f>
+              <c:f>Sheet1!$A$2:$C$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6.56574481348E6</c:v>
+                  <c:v>921911.314733769</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2488.66572260652</c:v>
+                  <c:v>662118.253708323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>922167.63393722</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -217,11 +236,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1403185600"/>
-        <c:axId val="-1437357600"/>
+        <c:axId val="1866219488"/>
+        <c:axId val="1866224032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1403185600"/>
+        <c:axId val="1866219488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -264,7 +283,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1437357600"/>
+        <c:crossAx val="1866224032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -272,7 +291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1437357600"/>
+        <c:axId val="1866224032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1403185600"/>
+        <c:crossAx val="1866219488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -974,16 +993,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1268,32 +1287,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>6565744.81348</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>921911.31473376905</v>
       </c>
-      <c r="B2" s="1">
-        <v>2488.6657226065199</v>
+      <c r="B2" s="3">
+        <v>662118.253708323</v>
+      </c>
+      <c r="C2" s="2">
+        <v>922167.63393721997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>